<commit_message>
feat: Gestão de Vendas
</commit_message>
<xml_diff>
--- a/transportadora.xlsx
+++ b/transportadora.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,20 +436,30 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Unnamed: 0.2</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Unnamed: 0</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Nome</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Loc_Central</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>CNPJ</t>
         </is>

</xml_diff>